<commit_message>
add button into excel file
</commit_message>
<xml_diff>
--- a/src/data.xlsx
+++ b/src/data.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\posmis\YandexDisk\Учеба\4 курс\Прочность конструкции\КР\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\chiquitv\Projects\wingConsoleStrenght\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BCB269-A9FC-48D4-804E-7F7DAD6DAE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D86345F-A66C-498C-8B0D-5191F36ADE4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="results" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>Вариант №16</t>
   </si>
@@ -235,13 +236,19 @@
   </si>
   <si>
     <t>Кол-во стрингеров и поясов лонжеронов</t>
+  </si>
+  <si>
+    <t>Номер стрингера</t>
+  </si>
+  <si>
+    <t>fi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +262,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="9">
@@ -402,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -419,45 +433,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -468,9 +482,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -488,6 +499,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Button" lockText="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,6 +551,76 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>12</xdr:col>
+          <xdr:colOff>276225</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>16</xdr:col>
+          <xdr:colOff>266700</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>104775</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Button 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="ctr" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Calibri"/>
+                  <a:ea typeface="Calibri"/>
+                  <a:cs typeface="Calibri"/>
+                </a:rPr>
+                <a:t>Кнопка 2</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData fPrintsWithSheet="0"/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -801,11 +886,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Лист1"/>
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,16 +941,16 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="22"/>
@@ -878,7 +964,7 @@
       <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B4" s="2">
@@ -897,7 +983,7 @@
       <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2">
@@ -914,19 +1000,19 @@
         <f>IF(J5,2,1)*$B$30+$B$12</f>
         <v>14.080000000000002</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*$B$22*I5)</f>
         <v>-10.5</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>0</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2">
@@ -943,17 +1029,17 @@
         <f t="shared" ref="G6:G14" si="0">IF(J6,2,1)*$B$30+$B$12</f>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*$B$22*I6)</f>
         <v>-9.8568750000000005</v>
       </c>
-      <c r="I6" s="12">
-        <v>1</v>
-      </c>
-      <c r="J6" s="16"/>
+      <c r="I6" s="11">
+        <v>1</v>
+      </c>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2">
@@ -970,17 +1056,17 @@
         <f t="shared" si="0"/>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*$B$22*I7)</f>
         <v>-9.213750000000001</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>2</v>
       </c>
-      <c r="J7" s="16"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="2">
@@ -997,17 +1083,17 @@
         <f t="shared" si="0"/>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*$B$22*I8)</f>
         <v>-8.5706249999999997</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="11">
         <v>3</v>
       </c>
-      <c r="J8" s="16"/>
+      <c r="J8" s="15"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="2">
@@ -1026,19 +1112,19 @@
         <f t="shared" si="0"/>
         <v>14.080000000000002</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*$B$22*I9)</f>
         <v>-7.9275000000000002</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="11">
         <v>4</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="2">
@@ -1057,17 +1143,17 @@
         <f t="shared" si="0"/>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*($B$22*$I$9+$B$23*I10))</f>
         <v>-6.9720000000000004</v>
       </c>
-      <c r="I10" s="13">
-        <v>1</v>
-      </c>
-      <c r="J10" s="16"/>
+      <c r="I10" s="12">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="2">
@@ -1086,17 +1172,17 @@
         <f t="shared" si="0"/>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*($B$22*$I$9+$B$23*I11))</f>
         <v>-6.0165000000000006</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <v>2</v>
       </c>
-      <c r="J11" s="16"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="2">
@@ -1115,17 +1201,17 @@
         <f t="shared" si="0"/>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*($B$22*$I$9+$B$23*I12))</f>
         <v>-5.0610000000000008</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="12">
         <v>3</v>
       </c>
-      <c r="J12" s="16"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="2">
@@ -1144,17 +1230,17 @@
         <f t="shared" si="0"/>
         <v>9.2800000000000011</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*($B$22*$I$9+$B$23*I13))</f>
         <v>-4.105500000000001</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="12">
         <v>4</v>
       </c>
-      <c r="J13" s="16"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="2">
@@ -1173,19 +1259,19 @@
         <f t="shared" si="0"/>
         <v>14.080000000000002</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <f>-($B$20/2-($B$20-$B$21)/$B$5*($B$22*$I$9+$B$23*I14))</f>
         <v>-3.1500000000000004</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>5</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2">
@@ -1206,13 +1292,13 @@
         <f>$B$20/2</f>
         <v>10.5</v>
       </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="16">
+      <c r="I15" s="9"/>
+      <c r="J15" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="2">
@@ -1233,11 +1319,11 @@
         <f t="shared" ref="H16:H24" si="2">$B$20/2</f>
         <v>10.5</v>
       </c>
-      <c r="I16" s="10"/>
-      <c r="J16" s="16"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="2">
@@ -1260,11 +1346,11 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I17" s="10"/>
-      <c r="J17" s="16"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="2">
@@ -1287,11 +1373,11 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="16"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="15"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="3">
@@ -1313,11 +1399,11 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="16"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="15"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="3">
@@ -1339,13 +1425,13 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="16">
+      <c r="I20" s="9"/>
+      <c r="J20" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="3">
@@ -1367,11 +1453,11 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="16"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B22" s="2">
@@ -1395,11 +1481,11 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="16"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B23" s="2">
@@ -1423,11 +1509,11 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="16"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1448,13 +1534,13 @@
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="17">
+      <c r="I24" s="9"/>
+      <c r="J24" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="2">
@@ -1467,7 +1553,7 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B26" s="2">
@@ -1480,7 +1566,7 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="2">
@@ -1493,7 +1579,7 @@
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="2">
@@ -1505,7 +1591,7 @@
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>47</v>
       </c>
       <c r="B29" s="2">
@@ -1517,7 +1603,7 @@
       <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B30" s="4">
@@ -1530,7 +1616,7 @@
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B31" s="4">
@@ -1543,7 +1629,7 @@
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B32" s="4">
@@ -1556,7 +1642,7 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B33" s="4">
@@ -1570,7 +1656,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="17" t="s">
         <v>66</v>
       </c>
       <c r="B34" s="4">
@@ -1603,5 +1689,223 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId4" name="Button 2">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!ЭтаКнига.RunPythonScript">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>12</xdr:col>
+                    <xdr:colOff>276225</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>16</xdr:col>
+                    <xdr:colOff>266700</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>104775</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA87B472-FA5A-433B-ADA0-DD85B12AC57E}">
+  <sheetPr codeName="Лист2"/>
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0.97342187108053602</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.99962796405578991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>